<commit_message>
Update and finalise tests
</commit_message>
<xml_diff>
--- a/tests/link_budget_validation.xlsx
+++ b/tests/link_budget_validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\digital_comms\tests\mobile_network\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\pysim5g\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC54474-61BD-45E8-B52C-368F9897F0FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51A1FDE-D384-4FEF-84C1-875779B663FE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="3480" windowWidth="21780" windowHeight="13035" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="link_buget_example 1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
   <si>
     <t>Rx Power (dBm)</t>
   </si>
@@ -224,16 +225,24 @@
   <si>
     <t>Area (km^2)</t>
   </si>
+  <si>
+    <t>Capacity (Mbps)</t>
+  </si>
+  <si>
+    <t>Capacity (bps/km2)</t>
+  </si>
+  <si>
+    <t>Capacity (Mbps/km2)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -317,7 +326,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -522,12 +531,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -647,6 +684,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -665,10 +705,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -986,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,7 +1076,7 @@
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <f>(B3+C3-D3)-E3-F3+G3-H3</f>
-        <v>-48.44</v>
+        <v>-57.989999999999995</v>
       </c>
       <c r="B3" s="6">
         <v>40</v>
@@ -1048,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="6">
-        <v>99.44</v>
+        <v>108.99</v>
       </c>
       <c r="F3" s="6">
         <v>4</v>
@@ -1099,7 +1139,7 @@
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27">
         <f>(B9+C9-D9)-E9-F9+G9-H9</f>
-        <v>-65.430000000000007</v>
+        <v>-59.86</v>
       </c>
       <c r="B9" s="28">
         <v>40</v>
@@ -1111,8 +1151,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="28">
-        <f>113.12+3.31</f>
-        <v>116.43</v>
+        <v>110.86</v>
       </c>
       <c r="F9" s="28">
         <v>4</v>
@@ -1165,7 +1204,7 @@
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27">
         <f>(B12+C12-D12)-E12-F12+G12-H12</f>
-        <v>-65.5</v>
+        <v>-59.86</v>
       </c>
       <c r="B12" s="28">
         <v>40</v>
@@ -1177,8 +1216,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="28">
-        <f>113.19+3.31</f>
-        <v>116.5</v>
+        <v>110.86</v>
       </c>
       <c r="F12" s="28">
         <v>4</v>
@@ -1231,7 +1269,7 @@
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>(B15+C15-D15)-E15-F15+G15-H15</f>
-        <v>-77.88</v>
+        <v>-69.98</v>
       </c>
       <c r="B15" s="6">
         <v>40</v>
@@ -1243,8 +1281,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="6">
-        <f>125.57+3.31</f>
-        <v>128.88</v>
+        <v>120.98</v>
       </c>
       <c r="F15" s="6">
         <v>4</v>
@@ -1342,11 +1379,11 @@
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <f>B25+C25</f>
-        <v>3.438814975570614E-66</v>
+        <v>1.3803842646552066E-60</v>
       </c>
       <c r="B25" s="13">
         <f>SUM(POWER(10, A9),POWER(10, A12),POWER(10, A15))*(D25/100)</f>
-        <v>3.438814975570614E-66</v>
+        <v>1.3803842646552066E-60</v>
       </c>
       <c r="C25" s="13">
         <f>POWER(10, A20)</f>
@@ -1375,15 +1412,15 @@
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <f>LOG10(B30/C30)</f>
-        <v>17.023591190636374</v>
+        <v>1.8699999999835324</v>
       </c>
       <c r="B30" s="13">
         <f>POWER(10,A3)</f>
-        <v>3.6307805477009909E-49</v>
+        <v>1.0232929922807394E-58</v>
       </c>
       <c r="C30" s="16">
         <f>A25</f>
-        <v>3.438814975570614E-66</v>
+        <v>1.3803842646552066E-60</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1401,53 +1438,107 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
-        <v>5.5547000000000004</v>
+        <v>1.4765999999999999</v>
       </c>
       <c r="B35" s="16">
         <f>A30</f>
-        <v>17.023591190636374</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+        <v>1.8699999999835324</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="21" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B38" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="39" t="s">
+      <c r="D38" s="39" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="23">
-        <f>B40*C40/D40</f>
-        <v>2169804687.5</v>
-      </c>
-      <c r="B40" s="30">
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="23">
+        <f>B39*C39</f>
+        <v>14766000</v>
+      </c>
+      <c r="B39" s="30">
         <f>A35</f>
-        <v>5.5547000000000004</v>
-      </c>
-      <c r="C40" s="49">
+        <v>1.4765999999999999</v>
+      </c>
+      <c r="C39" s="43">
+        <f>10000000</f>
+        <v>10000000</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0.21650630000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="51">
+        <f>A39/1000000</f>
+        <v>14.766</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="23">
+        <f>B46*C46/D46</f>
+        <v>68201248.647267997</v>
+      </c>
+      <c r="B46" s="30">
+        <f>A35</f>
+        <v>1.4765999999999999</v>
+      </c>
+      <c r="C46" s="43">
         <f>E20</f>
         <v>10000000</v>
       </c>
-      <c r="D40" s="7">
-        <v>2.5600000000000001E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="50">
-        <f>A40/1000000</f>
-        <v>2169.8046875</v>
+      <c r="D46" s="7">
+        <v>0.21650630000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="51">
+        <f>A46/1000000</f>
+        <v>68.201248647268002</v>
       </c>
     </row>
   </sheetData>
@@ -1476,25 +1567,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47" t="s">
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
+      <c r="A2" s="45"/>
       <c r="B2" s="31" t="s">
         <v>37</v>
       </c>
@@ -1513,7 +1604,7 @@
       <c r="G2" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="48"/>
+      <c r="H2" s="49"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="33">

</xml_diff>

<commit_message>
Add new 5G propagation model tests
</commit_message>
<xml_diff>
--- a/tests/link_budget_validation.xlsx
+++ b/tests/link_budget_validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\pysim5g\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51A1FDE-D384-4FEF-84C1-875779B663FE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A31091C-D60F-482D-9D35-F8545CCAC04C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="3480" windowWidth="21780" windowHeight="13035" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="14415" windowHeight="13290" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="link_buget_example 1" sheetId="1" r:id="rId1"/>
@@ -687,6 +687,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -704,12 +710,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,7 +1076,7 @@
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <f>(B3+C3-D3)-E3-F3+G3-H3</f>
-        <v>-57.989999999999995</v>
+        <v>-60</v>
       </c>
       <c r="B3" s="6">
         <v>40</v>
@@ -1088,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="6">
-        <v>108.99</v>
+        <v>111</v>
       </c>
       <c r="F3" s="6">
         <v>4</v>
@@ -1139,7 +1139,7 @@
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27">
         <f>(B9+C9-D9)-E9-F9+G9-H9</f>
-        <v>-59.86</v>
+        <v>-73</v>
       </c>
       <c r="B9" s="28">
         <v>40</v>
@@ -1151,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="28">
-        <v>110.86</v>
+        <v>124</v>
       </c>
       <c r="F9" s="28">
         <v>4</v>
@@ -1204,7 +1204,7 @@
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27">
         <f>(B12+C12-D12)-E12-F12+G12-H12</f>
-        <v>-59.86</v>
+        <v>-62</v>
       </c>
       <c r="B12" s="28">
         <v>40</v>
@@ -1216,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="28">
-        <v>110.86</v>
+        <v>113</v>
       </c>
       <c r="F12" s="28">
         <v>4</v>
@@ -1269,7 +1269,7 @@
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>(B15+C15-D15)-E15-F15+G15-H15</f>
-        <v>-69.98</v>
+        <v>-78</v>
       </c>
       <c r="B15" s="6">
         <v>40</v>
@@ -1281,7 +1281,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="6">
-        <v>120.98</v>
+        <v>129</v>
       </c>
       <c r="F15" s="6">
         <v>4</v>
@@ -1379,11 +1379,11 @@
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <f>B25+C25</f>
-        <v>1.3803842646552066E-60</v>
+        <v>5.0000000000500004E-63</v>
       </c>
       <c r="B25" s="13">
         <f>SUM(POWER(10, A9),POWER(10, A12),POWER(10, A15))*(D25/100)</f>
-        <v>1.3803842646552066E-60</v>
+        <v>5.0000000000500004E-63</v>
       </c>
       <c r="C25" s="13">
         <f>POWER(10, A20)</f>
@@ -1412,15 +1412,15 @@
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <f>LOG10(B30/C30)</f>
-        <v>1.8699999999835324</v>
+        <v>2.3010299956596381</v>
       </c>
       <c r="B30" s="13">
         <f>POWER(10,A3)</f>
-        <v>1.0232929922807394E-58</v>
+        <v>1.0000000000000001E-60</v>
       </c>
       <c r="C30" s="16">
         <f>A25</f>
-        <v>1.3803842646552066E-60</v>
+        <v>5.0000000000500004E-63</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="B35" s="16">
         <f>A30</f>
-        <v>1.8699999999835324</v>
+        <v>2.3010299956596381</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1483,12 +1483,12 @@
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="50" t="s">
+      <c r="A41" s="44" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="51">
+      <c r="A42" s="45">
         <f>A39/1000000</f>
         <v>14.766</v>
       </c>
@@ -1531,12 +1531,12 @@
     </row>
     <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="50" t="s">
+      <c r="A48" s="44" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="51">
+      <c r="A49" s="45">
         <f>A46/1000000</f>
         <v>68.201248647268002</v>
       </c>
@@ -1567,25 +1567,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47" t="s">
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48" t="s">
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
+      <c r="A2" s="47"/>
       <c r="B2" s="31" t="s">
         <v>37</v>
       </c>
@@ -1604,7 +1604,7 @@
       <c r="G2" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="49"/>
+      <c r="H2" s="51"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="33">

</xml_diff>